<commit_message>
List of variables and pca data
</commit_message>
<xml_diff>
--- a/List of variables.xlsx
+++ b/List of variables.xlsx
@@ -11,13 +11,15 @@
     <sheet name="Livestock" sheetId="1" r:id="rId2"/>
     <sheet name="MGNREGA" sheetId="3" r:id="rId3"/>
     <sheet name="Agcensus" sheetId="4" r:id="rId4"/>
+    <sheet name="Aphrodite" sheetId="5" r:id="rId5"/>
+    <sheet name="PCA-Amenities" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>No of Households</t>
   </si>
@@ -329,6 +331,114 @@
   </si>
   <si>
     <t>Food grains</t>
+  </si>
+  <si>
+    <t>Total female indigenous cattle</t>
+  </si>
+  <si>
+    <t>Percentage tree cover</t>
+  </si>
+  <si>
+    <t>Precipitation</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>Nightlights</t>
+  </si>
+  <si>
+    <t>Diary animals</t>
+  </si>
+  <si>
+    <t>Total female buffalo, Total female exotic cattle,  Total indigenous cattle in milk</t>
+  </si>
+  <si>
+    <t>Work Animals</t>
+  </si>
+  <si>
+    <t>Total male buffalo, Total male exotic cattle, female indigenous cattle excluding cattle in milk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of HH's using firewood for cooking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of HH's using LPG/PNG for cooking </t>
+  </si>
+  <si>
+    <t>% of HH's using Kerosone for cooking</t>
+  </si>
+  <si>
+    <t>% of HH's using crop residue for cooking</t>
+  </si>
+  <si>
+    <t>% of HH's availing banking services</t>
+  </si>
+  <si>
+    <t>% of HH's using television</t>
+  </si>
+  <si>
+    <t>% of HH's having computer laptop</t>
+  </si>
+  <si>
+    <t>% of HH's having mobile</t>
+  </si>
+  <si>
+    <t>% of HH's having cooking outside house</t>
+  </si>
+  <si>
+    <t>% of HH's having electricity as the main source of lighting</t>
+  </si>
+  <si>
+    <t>% of HH's having drinking water from treated tap water</t>
+  </si>
+  <si>
+    <t>% of HH's having drinking water from un-treated tap water</t>
+  </si>
+  <si>
+    <t>% of HH's having latrine facility within the premises</t>
+  </si>
+  <si>
+    <t>% of HH's having G.I./Metal/ Asbestos sheets under material of roof</t>
+  </si>
+  <si>
+    <t>% of HH's having Concrete under material of roof</t>
+  </si>
+  <si>
+    <t>% of HH's having Grass/ Thatch/ Bamboo/ Wood/Mud etc. under material of roof</t>
+  </si>
+  <si>
+    <t>% of HH's having Grass/ Thatch/ Bamboo/ Wood/Mud etc. under material of wall</t>
+  </si>
+  <si>
+    <t>% of HH's having Concrete under material of wall</t>
+  </si>
+  <si>
+    <t>% of HH's having G.I./Metal/ Asbestos sheets under material of wall</t>
+  </si>
+  <si>
+    <t>% of HH's having mud under material of floor</t>
+  </si>
+  <si>
+    <t>% of HH's having cement under material of floor</t>
+  </si>
+  <si>
+    <t>% of HH's having wood/bamboo under material of floor</t>
+  </si>
+  <si>
+    <t>% of HH's having different HH size (1,2,3,4,5,6-8, 9+)</t>
+  </si>
+  <si>
+    <t>% of HH's having drinking water within premises</t>
+  </si>
+  <si>
+    <t>% of HH's having drinking water near premises</t>
+  </si>
+  <si>
+    <t>% of HH's having drinking water away.</t>
   </si>
 </sst>
 </file>
@@ -488,7 +598,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -496,14 +606,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -518,13 +632,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -824,7 +942,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1038,61 +1158,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75">
+    <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75">
+    <row r="3" spans="1:2" ht="15.75">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75">
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75">
+    <row r="6" spans="1:2" ht="15.75">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:2" ht="15.75">
+      <c r="A7" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75">
+      <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:2" ht="15.75">
+      <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:2" ht="15.75">
+      <c r="A10" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75">
+      <c r="A11" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75">
+      <c r="A12" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1105,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1248,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1260,192 +1402,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5">
+      <c r="A1" s="11">
         <v>2011</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="18" t="s">
         <v>96</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75">
-      <c r="A7" s="16"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:3" ht="15.75">
-      <c r="A8" s="16"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3" ht="15.75">
-      <c r="A9" s="16"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:3" ht="15.75">
-      <c r="A10" s="16"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="16"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="16"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="16"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="15"/>
     </row>
     <row r="14" spans="1:3" ht="15.75">
-      <c r="A14" s="16"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="16" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75">
-      <c r="A15" s="16"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:3" ht="15.75">
-      <c r="A16" s="16"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3" ht="15.75">
-      <c r="A17" s="16"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:3" ht="15.75">
-      <c r="A18" s="16"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" ht="15.75">
-      <c r="A19" s="16"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3" ht="15.75">
-      <c r="A20" s="16"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:3" ht="15.75">
-      <c r="A21" s="16"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:3" ht="15.75">
-      <c r="A22" s="16"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" ht="15.75">
-      <c r="A23" s="16"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="8"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="18"/>
+      <c r="B26" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="8"/>
+      <c r="C26" s="17"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="15" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1458,4 +1600,197 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75">
+      <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75">
+      <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75">
+      <c r="A3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75">
+      <c r="A4" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75">
+      <c r="A5" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="74.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75">
+      <c r="A1" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75">
+      <c r="A2" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75">
+      <c r="A3" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75">
+      <c r="A4" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75">
+      <c r="A6" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75">
+      <c r="A7" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75">
+      <c r="A8" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75">
+      <c r="A9" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75">
+      <c r="A10" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75">
+      <c r="A11" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75">
+      <c r="A12" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75">
+      <c r="A13" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75">
+      <c r="A14" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75">
+      <c r="A15" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75">
+      <c r="A16" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75">
+      <c r="A17" s="20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75">
+      <c r="A18" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75">
+      <c r="A19" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75">
+      <c r="A20" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75">
+      <c r="A21" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75">
+      <c r="A22" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75">
+      <c r="A23" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75">
+      <c r="A24" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75">
+      <c r="A25" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75">
+      <c r="A26" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added PMGSY, Livestock statewise report
</commit_message>
<xml_diff>
--- a/List of variables.xlsx
+++ b/List of variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20055" windowHeight="7935" tabRatio="750" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Primary census Abstract" sheetId="2" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Agcensus" sheetId="4" r:id="rId4"/>
     <sheet name="Aphrodite" sheetId="5" r:id="rId5"/>
     <sheet name="PCA-Amenities" sheetId="6" r:id="rId6"/>
+    <sheet name="PMGSY" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="297">
   <si>
     <t>No of Households</t>
   </si>
@@ -54,9 +55,6 @@
     <t>Total Work Population</t>
   </si>
   <si>
-    <t>Total Male Work Population</t>
-  </si>
-  <si>
     <t>Total Female work Population</t>
   </si>
   <si>
@@ -439,13 +437,487 @@
   </si>
   <si>
     <t>% of HH's having drinking water away.</t>
+  </si>
+  <si>
+    <t>Total Male work Population</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Geographical Unit</t>
+  </si>
+  <si>
+    <t>Routes</t>
+  </si>
+  <si>
+    <t>Batches</t>
+  </si>
+  <si>
+    <t>Years Available</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Collaborations</t>
+  </si>
+  <si>
+    <t>Core Network</t>
+  </si>
+  <si>
+    <t>CNCPL (Core Network New Connectivity Priority List)</t>
+  </si>
+  <si>
+    <t>Road Number</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Link, Through, All</t>
+  </si>
+  <si>
+    <t>Road Name</t>
+  </si>
+  <si>
+    <t>Road Route</t>
+  </si>
+  <si>
+    <t>Partial/Full Length</t>
+  </si>
+  <si>
+    <t>Road Length</t>
+  </si>
+  <si>
+    <t>Road From</t>
+  </si>
+  <si>
+    <t>Road To</t>
+  </si>
+  <si>
+    <t>Target Habitation</t>
+  </si>
+  <si>
+    <t>Total Population Served</t>
+  </si>
+  <si>
+    <t>CUPL (Core Network Upgradation Priority List)</t>
+  </si>
+  <si>
+    <t>Year of Construction</t>
+  </si>
+  <si>
+    <t>Year of Last Periodic Renewal</t>
+  </si>
+  <si>
+    <t>Total Population of the Habitation Served</t>
+  </si>
+  <si>
+    <t>Average Annual Daily Traffic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year </t>
+  </si>
+  <si>
+    <t>Average PCI</t>
+  </si>
+  <si>
+    <t>Pavement Condition Index</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Segment Number</t>
+  </si>
+  <si>
+    <t>Start Chainage</t>
+  </si>
+  <si>
+    <t>End Chainage</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Habitation Wise Core Network</t>
+  </si>
+  <si>
+    <t>Habitation Name</t>
+  </si>
+  <si>
+    <t>From Chainage</t>
+  </si>
+  <si>
+    <t>To Chainage</t>
+  </si>
+  <si>
+    <t>Road Wise Core Network</t>
+  </si>
+  <si>
+    <t>Road From Chainage</t>
+  </si>
+  <si>
+    <t>Road To Chainage</t>
+  </si>
+  <si>
+    <t>Habitation Population</t>
+  </si>
+  <si>
+    <t>Proposals</t>
+  </si>
+  <si>
+    <t>Sanctioned Projects</t>
+  </si>
+  <si>
+    <t>No. of Packages</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>1 Through 5</t>
+  </si>
+  <si>
+    <t>2001 to 2015</t>
+  </si>
+  <si>
+    <t>Total No. of Proposals</t>
+  </si>
+  <si>
+    <t>Collaboration_ADB (PMGSY)</t>
+  </si>
+  <si>
+    <t>Collaboration_Regular (PMGSY)</t>
+  </si>
+  <si>
+    <t>Collaboration_World Bank (RRP-1)</t>
+  </si>
+  <si>
+    <t>Collaboration_World Bank (RRP-2)</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>No. of Habitations Covered</t>
+  </si>
+  <si>
+    <t>No. of Roads</t>
+  </si>
+  <si>
+    <t>Total Length</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Cost Per Km</t>
+  </si>
+  <si>
+    <t>No. of CD Works</t>
+  </si>
+  <si>
+    <t>CD Works Cost</t>
+  </si>
+  <si>
+    <t>No. of LSB (Long Span Bridge) Works</t>
+  </si>
+  <si>
+    <t>LSB Cost</t>
+  </si>
+  <si>
+    <t>Protection Cost</t>
+  </si>
+  <si>
+    <t>Other Cost</t>
+  </si>
+  <si>
+    <t>State Cost</t>
+  </si>
+  <si>
+    <t>Pending Proposals</t>
+  </si>
+  <si>
+    <t>Variables Upto Block Level</t>
+  </si>
+  <si>
+    <t>Proposals Prepared by DPIU (District Programme Implementation Unit)</t>
+  </si>
+  <si>
+    <t>No. of Proposals</t>
+  </si>
+  <si>
+    <t>Cost (State Share)</t>
+  </si>
+  <si>
+    <t>Proposal Cost</t>
+  </si>
+  <si>
+    <t>Proposals Pending for clearance by STA and MoRD Both</t>
+  </si>
+  <si>
+    <t>Proposal Pending for Clearance by MoRD</t>
+  </si>
+  <si>
+    <t>Variables For a Block</t>
+  </si>
+  <si>
+    <t>Sanctioned Year</t>
+  </si>
+  <si>
+    <t>Package No.</t>
+  </si>
+  <si>
+    <t>Road/Bridge Name</t>
+  </si>
+  <si>
+    <t>Proposal Type</t>
+  </si>
+  <si>
+    <t>New/Upgrade</t>
+  </si>
+  <si>
+    <t>Proposal Stage</t>
+  </si>
+  <si>
+    <t>Proposal Length</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Phasewise Per Kilometer Cost</t>
+  </si>
+  <si>
+    <t>Per Kilomete Cost For a Upgradation/New Connectivity Year 2001-2007</t>
+  </si>
+  <si>
+    <t>Variables for a Block</t>
+  </si>
+  <si>
+    <t>Package Name</t>
+  </si>
+  <si>
+    <t>Collaboration</t>
+  </si>
+  <si>
+    <t>Pavement Length</t>
+  </si>
+  <si>
+    <t>Pavement Cost</t>
+  </si>
+  <si>
+    <t>Maintenance Cost</t>
+  </si>
+  <si>
+    <t>State Wise List of Roads</t>
+  </si>
+  <si>
+    <t>In Progress, Complete, All</t>
+  </si>
+  <si>
+    <t>ADB (PMGSY), Regular PMGSY, World Bank (RRP-1), World Bank (RRP-2)</t>
+  </si>
+  <si>
+    <t>Total Road Length</t>
+  </si>
+  <si>
+    <t>Total Payment Made</t>
+  </si>
+  <si>
+    <t>Road Name/Bridge Name</t>
+  </si>
+  <si>
+    <t>Connectivity (New/Upgrade)</t>
+  </si>
+  <si>
+    <t>Name of Benefited Habitation</t>
+  </si>
+  <si>
+    <t>Sanctioned Cost</t>
+  </si>
+  <si>
+    <t>Road Length (Km)/Bridge Length (M)</t>
+  </si>
+  <si>
+    <t>Expenditure Till Date</t>
+  </si>
+  <si>
+    <t>State of Progress</t>
+  </si>
+  <si>
+    <t>Contractor Name</t>
+  </si>
+  <si>
+    <t>5 Years Maintenance Cost Due</t>
+  </si>
+  <si>
+    <t>Year Wise Maintenance Expenditure</t>
+  </si>
+  <si>
+    <t>Completion Date</t>
+  </si>
+  <si>
+    <t>Completed Road With Value of Work Done</t>
+  </si>
+  <si>
+    <t>Variables upto Block Level</t>
+  </si>
+  <si>
+    <t>Value of Work Done</t>
+  </si>
+  <si>
+    <t>Payment Made</t>
+  </si>
+  <si>
+    <t>Name of Road</t>
+  </si>
+  <si>
+    <t>Physical Progress</t>
+  </si>
+  <si>
+    <t>Habitation Coverage</t>
+  </si>
+  <si>
+    <t>Total No. of Habitations</t>
+  </si>
+  <si>
+    <t>Unconnected as on 01-04-200</t>
+  </si>
+  <si>
+    <t>Covered (Sanctioned under PMGSY) 11-09-2014</t>
+  </si>
+  <si>
+    <t>Covered Under State Schemes (11-09-2014)</t>
+  </si>
+  <si>
+    <t>Balance (11-09-2014)</t>
+  </si>
+  <si>
+    <t>Demographics, School, Health, other infrastructure</t>
+  </si>
+  <si>
+    <t>Physical Progress of Works</t>
+  </si>
+  <si>
+    <t>Road Works Sanctioned</t>
+  </si>
+  <si>
+    <t>Completed Works</t>
+  </si>
+  <si>
+    <t>Ongoing Works</t>
+  </si>
+  <si>
+    <t>Completed Length of Ongoing Works</t>
+  </si>
+  <si>
+    <t>Total Completed Length</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Upgrade/New</t>
+  </si>
+  <si>
+    <t>Surface Type</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>pavement Cost</t>
+  </si>
+  <si>
+    <t>LSB State Cost</t>
+  </si>
+  <si>
+    <t>Protection Work</t>
+  </si>
+  <si>
+    <t>Other Works</t>
+  </si>
+  <si>
+    <t>Present Status</t>
+  </si>
+  <si>
+    <t>Completed Length</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>SC/ST Population</t>
+  </si>
+  <si>
+    <t>Completed Roads</t>
+  </si>
+  <si>
+    <t>Total Number of Proposals</t>
+  </si>
+  <si>
+    <t>Sanctinoed Cost</t>
+  </si>
+  <si>
+    <t>Road/Bridge Length</t>
+  </si>
+  <si>
+    <t>Financial Completion Month/Year</t>
+  </si>
+  <si>
+    <t>Road Wise Progress of Work</t>
+  </si>
+  <si>
+    <t>Total No. of Roads</t>
+  </si>
+  <si>
+    <t>Road Cost</t>
+  </si>
+  <si>
+    <t>Sanction Year</t>
+  </si>
+  <si>
+    <t>Work Award Date</t>
+  </si>
+  <si>
+    <t>Stipulated Date of Completion</t>
+  </si>
+  <si>
+    <t>Actual Date of Completion</t>
+  </si>
+  <si>
+    <t>Completion Status</t>
+  </si>
+  <si>
+    <t>State Road Completion Report</t>
+  </si>
+  <si>
+    <t>Agreement Cost</t>
+  </si>
+  <si>
+    <t>Date of Award</t>
+  </si>
+  <si>
+    <t>Due Date of Completion</t>
+  </si>
+  <si>
+    <t>Contractor Company Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,6 +963,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -598,7 +1078,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -614,6 +1094,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -638,12 +1124,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -942,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1008,147 +1497,147 @@
     </row>
     <row r="12" spans="1:1" ht="15.75">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1173,68 +1662,68 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75">
       <c r="A7" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75">
       <c r="A11" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75">
       <c r="A12" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1247,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -1258,127 +1747,127 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75">
       <c r="A5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75">
       <c r="A6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75">
       <c r="A7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75">
       <c r="A9" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75">
       <c r="A10" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75">
       <c r="A12" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75">
       <c r="A13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75">
       <c r="A14" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75">
       <c r="A15" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75">
       <c r="A16" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75">
       <c r="A17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75">
       <c r="A18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75">
       <c r="A19" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75">
       <c r="A20" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75">
       <c r="A21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75">
       <c r="A22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75">
       <c r="A23" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75">
       <c r="A24" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75">
       <c r="A25" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1390,7 +1879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -1402,192 +1891,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="11">
+      <c r="A1" s="13">
         <v>2011</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="5" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="14"/>
+      <c r="B4" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A6" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="20"/>
+      <c r="B7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75">
+      <c r="A8" s="20"/>
+      <c r="B8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="16"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="A9" s="20"/>
+      <c r="B9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75">
+      <c r="A10" s="20"/>
+      <c r="B10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75">
+      <c r="A11" s="20"/>
+      <c r="B11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="16"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75">
+      <c r="A12" s="20"/>
+      <c r="B12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="16"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75">
+      <c r="A13" s="20"/>
+      <c r="B13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75">
+      <c r="A14" s="20"/>
+      <c r="B14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="20"/>
+      <c r="B15" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
-      <c r="A7" s="18"/>
-      <c r="B7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="14"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75">
-      <c r="A8" s="18"/>
-      <c r="B8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:3" ht="15.75">
-      <c r="A9" s="18"/>
-      <c r="B9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="14"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75">
-      <c r="A10" s="18"/>
-      <c r="B10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="14"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="18"/>
-      <c r="B11" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="14"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="18"/>
-      <c r="B12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="18"/>
-      <c r="B13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75">
-      <c r="A14" s="18"/>
-      <c r="B14" s="2" t="s">
+      <c r="C15" s="18"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="A16" s="20"/>
+      <c r="B16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="18"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75">
+      <c r="A17" s="20"/>
+      <c r="B17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="18"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75">
+      <c r="A18" s="20"/>
+      <c r="B18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75">
+      <c r="A19" s="20"/>
+      <c r="B19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C19" s="18"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75">
+      <c r="A20" s="20"/>
+      <c r="B20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="18"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75">
+      <c r="A21" s="20"/>
+      <c r="B21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="18"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75">
+      <c r="A22" s="20"/>
+      <c r="B22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="18"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75">
+      <c r="A23" s="20"/>
+      <c r="B23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="18"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="20"/>
+      <c r="B24" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75">
-      <c r="A15" s="18"/>
-      <c r="B15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="16"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75">
-      <c r="A16" s="18"/>
-      <c r="B16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="16"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.75">
-      <c r="A17" s="18"/>
-      <c r="B17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="16"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75">
-      <c r="A18" s="18"/>
-      <c r="B18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="16"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75">
-      <c r="A19" s="18"/>
-      <c r="B19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="16"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75">
-      <c r="A20" s="18"/>
-      <c r="B20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="16"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75">
-      <c r="A21" s="18"/>
-      <c r="B21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="16"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75">
-      <c r="A22" s="18"/>
-      <c r="B22" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" s="16"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75">
-      <c r="A23" s="18"/>
-      <c r="B23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="16"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="20"/>
+      <c r="B25" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="19"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="20"/>
+      <c r="B26" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="20"/>
+      <c r="B27" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1617,27 +2106,27 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1650,7 +2139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection sqref="A1:A26"/>
     </sheetView>
   </sheetViews>
@@ -1661,132 +2150,1498 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75">
       <c r="A1" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75">
       <c r="A2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75">
       <c r="A6" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75">
       <c r="A12" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75">
+      <c r="A15" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75">
-      <c r="A15" s="19" t="s">
+    <row r="16" spans="1:1" ht="15.75">
+      <c r="A16" s="12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75">
-      <c r="A16" s="20" t="s">
-        <v>126</v>
-      </c>
-    </row>
     <row r="17" spans="1:1" ht="15.75">
-      <c r="A17" s="20" t="s">
-        <v>114</v>
+      <c r="A17" s="12" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75">
       <c r="A18" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75">
+      <c r="A19" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75">
+      <c r="A20" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75">
-      <c r="A19" s="20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75">
-      <c r="A20" s="19" t="s">
+    <row r="21" spans="1:1" ht="15.75">
+      <c r="A21" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75">
-      <c r="A21" s="19" t="s">
+    <row r="22" spans="1:1" ht="15.75">
+      <c r="A22" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75">
-      <c r="A22" s="19" t="s">
+    <row r="23" spans="1:1" ht="15.75">
+      <c r="A23" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.75">
-      <c r="A23" s="19" t="s">
+    <row r="24" spans="1:1" ht="15.75">
+      <c r="A24" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75">
-      <c r="A24" s="19" t="s">
+    <row r="25" spans="1:1" ht="15.75">
+      <c r="A25" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.75">
-      <c r="A25" s="19" t="s">
+    <row r="26" spans="1:1" ht="15.75">
+      <c r="A26" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15.75">
-      <c r="A26" s="19" t="s">
-        <v>123</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I250"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="4" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30">
+      <c r="A2" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="24"/>
+      <c r="C3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="24"/>
+      <c r="C4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="24"/>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" s="24"/>
+      <c r="C6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" s="24"/>
+      <c r="C7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="24"/>
+      <c r="C8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="24"/>
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="24"/>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="24"/>
+      <c r="C11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="24"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="C14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="C15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="C16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="C17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="C18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="C19" s="21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="C20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="C21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="C22" s="21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="C23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="C24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="C25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="C26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="C27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="C32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="C33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="C34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="C35" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="C36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="C37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="C38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="C39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="C40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="C44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="C45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="C46" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="C47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="C48" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="C49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="C50" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="C51" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="C52" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="C53" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>183</v>
+      </c>
+      <c r="B56" t="s">
+        <v>184</v>
+      </c>
+      <c r="C56" t="s">
+        <v>185</v>
+      </c>
+      <c r="D56" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" t="s">
+        <v>186</v>
+      </c>
+      <c r="F56" t="s">
+        <v>187</v>
+      </c>
+      <c r="G56" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="C57" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="C58" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="C59" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="C60" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="C61" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="C62" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="C63" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="C64" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7">
+      <c r="C65" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7">
+      <c r="C66" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7">
+      <c r="C67" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7">
+      <c r="C68" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7">
+      <c r="C69" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7">
+      <c r="C70" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="C71" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="C72" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="C73" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="C74" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7">
+      <c r="C75" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7">
+      <c r="B77" t="s">
+        <v>207</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="D77" t="s">
+        <v>152</v>
+      </c>
+      <c r="E77" t="s">
+        <v>186</v>
+      </c>
+      <c r="F77" t="s">
+        <v>187</v>
+      </c>
+      <c r="G77" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7">
+      <c r="C78" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7">
+      <c r="C79" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7">
+      <c r="C80" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82" s="21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3">
+      <c r="C83" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3">
+      <c r="C84" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3">
+      <c r="C85" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3">
+      <c r="C86" s="21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3">
+      <c r="C87" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3">
+      <c r="C88" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3">
+      <c r="C89" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3">
+      <c r="C91" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3">
+      <c r="C92" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3">
+      <c r="C94" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3">
+      <c r="C95" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3">
+      <c r="C96" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="C97" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="C98" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="C99" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="C100" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="B104" t="s">
+        <v>224</v>
+      </c>
+      <c r="C104" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="C105" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="C107" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="C108" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="C109" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="C110" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="C111" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="C112" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9">
+      <c r="C113" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9">
+      <c r="C114" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9">
+      <c r="C115" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9">
+      <c r="C116" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9">
+      <c r="C117" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9">
+      <c r="B119" t="s">
+        <v>232</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="D119" t="s">
+        <v>152</v>
+      </c>
+      <c r="E119" t="s">
+        <v>186</v>
+      </c>
+      <c r="F119" t="s">
+        <v>187</v>
+      </c>
+      <c r="G119" t="s">
+        <v>188</v>
+      </c>
+      <c r="H119" t="s">
+        <v>233</v>
+      </c>
+      <c r="I119" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9">
+      <c r="C120" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9">
+      <c r="C121" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9">
+      <c r="C122" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9">
+      <c r="C123" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9">
+      <c r="C124" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9">
+      <c r="C126" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="127" spans="2:9">
+      <c r="C127" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9">
+      <c r="C128" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="129" spans="2:9">
+      <c r="C129" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="130" spans="2:9">
+      <c r="C130" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="131" spans="2:9">
+      <c r="C131" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="132" spans="2:9">
+      <c r="C132" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="133" spans="2:9">
+      <c r="C133" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="134" spans="2:9">
+      <c r="C134" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="135" spans="2:9">
+      <c r="C135" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="136" spans="2:9">
+      <c r="C136" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="137" spans="2:9">
+      <c r="C137" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="138" spans="2:9">
+      <c r="C138" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9">
+      <c r="C139" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="140" spans="2:9">
+      <c r="C140" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="141" spans="2:9">
+      <c r="C141" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="143" spans="2:9">
+      <c r="B143" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="C143" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D143" t="s">
+        <v>152</v>
+      </c>
+      <c r="E143" t="s">
+        <v>186</v>
+      </c>
+      <c r="F143" t="s">
+        <v>186</v>
+      </c>
+      <c r="G143" t="s">
+        <v>188</v>
+      </c>
+      <c r="H143" t="s">
+        <v>186</v>
+      </c>
+      <c r="I143" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="144" spans="2:9">
+      <c r="C144" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3">
+      <c r="C145" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3">
+      <c r="C146" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3">
+      <c r="C147" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3">
+      <c r="C148" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3">
+      <c r="C149" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3">
+      <c r="C151" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="152" spans="3:3">
+      <c r="C152" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="153" spans="3:3">
+      <c r="C153" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="154" spans="3:3">
+      <c r="C154" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3">
+      <c r="C155" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="156" spans="3:3">
+      <c r="C156" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="157" spans="3:3">
+      <c r="C157" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="158" spans="3:3">
+      <c r="C158" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="159" spans="3:3">
+      <c r="C159" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9">
+      <c r="A161" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="B161" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="C161" s="21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
+      <c r="C162" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
+      <c r="C163" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
+      <c r="C164" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="C165" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
+      <c r="C166" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9">
+      <c r="C168" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
+      <c r="C169" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="B171" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="C171" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D171" t="s">
+        <v>152</v>
+      </c>
+      <c r="E171" t="s">
+        <v>186</v>
+      </c>
+      <c r="F171" t="s">
+        <v>186</v>
+      </c>
+      <c r="G171" t="s">
+        <v>188</v>
+      </c>
+      <c r="H171" t="s">
+        <v>186</v>
+      </c>
+      <c r="I171" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="C172" s="25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="C173" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="C174" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="C175" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="C176" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3">
+      <c r="C177" s="21"/>
+    </row>
+    <row r="178" spans="3:3">
+      <c r="C178" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3">
+      <c r="C179" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="180" spans="3:3">
+      <c r="C180" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3">
+      <c r="C181" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="182" spans="3:3">
+      <c r="C182" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="183" spans="3:3">
+      <c r="C183" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="184" spans="3:3">
+      <c r="C184" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="185" spans="3:3">
+      <c r="C185" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="186" spans="3:3">
+      <c r="C186" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="187" spans="3:3">
+      <c r="C187" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="188" spans="3:3">
+      <c r="C188" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="189" spans="3:3">
+      <c r="C189" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="190" spans="3:3">
+      <c r="C190" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="191" spans="3:3">
+      <c r="C191" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="192" spans="3:3">
+      <c r="C192" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="193" spans="2:9">
+      <c r="C193" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="194" spans="2:9">
+      <c r="C194" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="195" spans="2:9">
+      <c r="C195" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="196" spans="2:9">
+      <c r="C196" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="197" spans="2:9">
+      <c r="C197" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="198" spans="2:9">
+      <c r="C198" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="200" spans="2:9">
+      <c r="B200" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="C200" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D200" t="s">
+        <v>152</v>
+      </c>
+      <c r="E200" t="s">
+        <v>186</v>
+      </c>
+      <c r="F200" t="s">
+        <v>186</v>
+      </c>
+      <c r="G200" t="s">
+        <v>188</v>
+      </c>
+      <c r="H200" t="s">
+        <v>186</v>
+      </c>
+      <c r="I200" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="201" spans="2:9">
+      <c r="C201" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="202" spans="2:9">
+      <c r="C202" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="203" spans="2:9">
+      <c r="C203" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="204" spans="2:9">
+      <c r="C204" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="205" spans="2:9">
+      <c r="C205" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="207" spans="2:9">
+      <c r="C207" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="208" spans="2:9">
+      <c r="C208" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9">
+      <c r="C209" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="210" spans="2:9">
+      <c r="C210" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="211" spans="2:9">
+      <c r="C211" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="212" spans="2:9">
+      <c r="C212" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="213" spans="2:9">
+      <c r="C213" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="214" spans="2:9">
+      <c r="C214" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="215" spans="2:9">
+      <c r="C215" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="217" spans="2:9">
+      <c r="B217" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="C217" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D217" t="s">
+        <v>152</v>
+      </c>
+      <c r="E217" t="s">
+        <v>186</v>
+      </c>
+      <c r="F217" t="s">
+        <v>186</v>
+      </c>
+      <c r="G217" t="s">
+        <v>188</v>
+      </c>
+      <c r="H217" t="s">
+        <v>186</v>
+      </c>
+      <c r="I217" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="218" spans="2:9">
+      <c r="C218" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="219" spans="2:9">
+      <c r="C219" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="220" spans="2:9">
+      <c r="C220" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="221" spans="2:9">
+      <c r="C221" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="223" spans="2:9">
+      <c r="C223" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="224" spans="2:9">
+      <c r="C224" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="225" spans="2:3">
+      <c r="C225" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="226" spans="2:3">
+      <c r="C226" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="227" spans="2:3">
+      <c r="C227" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="228" spans="2:3">
+      <c r="C228" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="229" spans="2:3">
+      <c r="C229" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="230" spans="2:3">
+      <c r="C230" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="231" spans="2:3">
+      <c r="C231" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="232" spans="2:3">
+      <c r="C232" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="234" spans="2:3">
+      <c r="B234" t="s">
+        <v>292</v>
+      </c>
+      <c r="C234" s="21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="235" spans="2:3">
+      <c r="C235" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="236" spans="2:3">
+      <c r="C236" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="237" spans="2:3">
+      <c r="C237" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="238" spans="2:3">
+      <c r="C238" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="240" spans="2:3">
+      <c r="C240" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="241" spans="3:3">
+      <c r="C241" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="242" spans="3:3">
+      <c r="C242" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="243" spans="3:3">
+      <c r="C243" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="244" spans="3:3">
+      <c r="C244" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="245" spans="3:3">
+      <c r="C245" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="246" spans="3:3">
+      <c r="C246" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="247" spans="3:3">
+      <c r="C247" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="248" spans="3:3">
+      <c r="C248" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="249" spans="3:3">
+      <c r="C249" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="250" spans="3:3">
+      <c r="C250" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added document of PMSY, add new variables in the list
</commit_message>
<xml_diff>
--- a/List of variables.xlsx
+++ b/List of variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="309">
   <si>
     <t>No of Households</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Total households reached 100 day limit</t>
   </si>
   <si>
-    <t>Total persons with disability</t>
-  </si>
-  <si>
     <t>Total households worked (non-SC/ST)</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>Net Area (in Ha.)Cultivated</t>
   </si>
   <si>
-    <t>Land (in Ha.)not Availablefor Cultivation</t>
-  </si>
-  <si>
     <t>Total Numberof Wells in Use (WithOut Pumpsets )</t>
   </si>
   <si>
@@ -592,18 +586,6 @@
     <t>Total No. of Proposals</t>
   </si>
   <si>
-    <t>Collaboration_ADB (PMGSY)</t>
-  </si>
-  <si>
-    <t>Collaboration_Regular (PMGSY)</t>
-  </si>
-  <si>
-    <t>Collaboration_World Bank (RRP-1)</t>
-  </si>
-  <si>
-    <t>Collaboration_World Bank (RRP-2)</t>
-  </si>
-  <si>
     <t>Others</t>
   </si>
   <si>
@@ -628,9 +610,6 @@
     <t>CD Works Cost</t>
   </si>
   <si>
-    <t>No. of LSB (Long Span Bridge) Works</t>
-  </si>
-  <si>
     <t>LSB Cost</t>
   </si>
   <si>
@@ -790,9 +769,6 @@
     <t>Total No. of Habitations</t>
   </si>
   <si>
-    <t>Unconnected as on 01-04-200</t>
-  </si>
-  <si>
     <t>Covered (Sanctioned under PMGSY) 11-09-2014</t>
   </si>
   <si>
@@ -911,13 +887,73 @@
   </si>
   <si>
     <t>Contractor Company Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A “muster roll” is essentially a labour attendance register, pertaining to a particular worksite and a particular period (e.g. two weeks). It is also used as a receipt, to claim funds from the Programme Officer for the payment of wages. </t>
+  </si>
+  <si>
+    <t>Land (in Ha.)not Available for Cultivation</t>
+  </si>
+  <si>
+    <t>% of HH's having  the condition of census house as livable</t>
+  </si>
+  <si>
+    <t>% of HH's having  the condition of census house as dilapidated</t>
+  </si>
+  <si>
+    <t>% of HH's having  the condition of census house as good</t>
+  </si>
+  <si>
+    <t>% HH's to the total households</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of HH's having residence under rent </t>
+  </si>
+  <si>
+    <t>% of HH's having residence under owned</t>
+  </si>
+  <si>
+    <t>% of HH's haivng Scooter/ Motorcycle/Moped</t>
+  </si>
+  <si>
+    <t>% f HH's having Car/ Jeep/Van</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of HH's having TV, Computer/Laptop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Pavement Condition Index rates the condition of the surface of a road network. </t>
+  </si>
+  <si>
+    <t>No of proposals under collaboration_ADB (PMGSY)</t>
+  </si>
+  <si>
+    <t>No of proposals Collaboration_Regular (PMGSY)</t>
+  </si>
+  <si>
+    <t>No of proposals under Collaboration_World Bank (RRP-1)</t>
+  </si>
+  <si>
+    <t>no of proposals under Collaboration_World Bank (RRP-2)</t>
+  </si>
+  <si>
+    <t>No. of cross drainage Works</t>
+  </si>
+  <si>
+    <t>No. of  Works under LSB (Long Span Bridge)</t>
+  </si>
+  <si>
+    <t>Unconnected as on 01-04-2000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -954,17 +990,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -981,7 +1006,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1072,25 +1097,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1100,6 +1128,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1124,15 +1161,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1431,9 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1497,7 +1534,7 @@
     </row>
     <row r="12" spans="1:1" ht="15.75">
       <c r="A12" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75">
@@ -1691,8 +1728,8 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75">
-      <c r="A7" s="9" t="s">
-        <v>103</v>
+      <c r="A7" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75">
@@ -1711,19 +1748,19 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75">
+      <c r="A12" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="6" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75">
-      <c r="A12" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1734,93 +1771,108 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75">
+    <row r="1" spans="1:13" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75">
+    <row r="2" spans="1:13" ht="15.75">
       <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75">
+      <c r="A4" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75">
-      <c r="A4" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.75">
+    <row r="5" spans="1:13" ht="15.75">
       <c r="A5" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75">
+    <row r="6" spans="1:13" ht="15.75">
       <c r="A6" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75">
+    <row r="8" spans="1:13" ht="15.75">
       <c r="A8" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75">
+    <row r="9" spans="1:13" ht="15.75">
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75">
+    <row r="10" spans="1:13" ht="15.75">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.75">
+      <c r="B10" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75">
       <c r="A11" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.75">
+      <c r="B11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75">
       <c r="A12" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75">
+    <row r="13" spans="1:13" ht="15.75">
       <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75">
+    <row r="14" spans="1:13" ht="15.75">
       <c r="A14" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75">
+    <row r="15" spans="1:13" ht="15.75">
       <c r="A15" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75">
+    <row r="16" spans="1:13" ht="15.75">
       <c r="A16" s="4" t="s">
         <v>61</v>
       </c>
@@ -1865,13 +1917,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.75">
-      <c r="A25" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:M10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1880,7 +1931,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B27" sqref="B1:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1890,193 +1941,196 @@
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="13">
+    <row r="1" spans="1:3" ht="15.75">
+      <c r="A1" s="14">
         <v>2011</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="15"/>
+      <c r="B2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75">
+      <c r="A3" s="15"/>
+      <c r="B3" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="5" t="s">
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="15"/>
+      <c r="B4" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A6" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="21"/>
+      <c r="B7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75">
+      <c r="A8" s="21"/>
+      <c r="B8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="A9" s="21"/>
+      <c r="B9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75">
+      <c r="A10" s="21"/>
+      <c r="B10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75">
+      <c r="A11" s="21"/>
+      <c r="B11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75">
+      <c r="A12" s="21"/>
+      <c r="B12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75">
+      <c r="A13" s="21"/>
+      <c r="B13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="18"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75">
+      <c r="A14" s="21"/>
+      <c r="B14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="21"/>
+      <c r="B15" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="A16" s="21"/>
+      <c r="B16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75">
+      <c r="A17" s="21"/>
+      <c r="B17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75">
+      <c r="A18" s="21"/>
+      <c r="B18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75">
+      <c r="A19" s="21"/>
+      <c r="B19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="19"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75">
+      <c r="A20" s="21"/>
+      <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="19"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75">
+      <c r="A21" s="21"/>
+      <c r="B21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="19"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75">
+      <c r="A22" s="21"/>
+      <c r="B22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="19"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75">
+      <c r="A23" s="21"/>
+      <c r="B23" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C23" s="19"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75">
+      <c r="A24" s="21"/>
+      <c r="B24" s="24" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
-      <c r="A7" s="20"/>
-      <c r="B7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="16"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75">
-      <c r="A8" s="20"/>
-      <c r="B8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="16"/>
-    </row>
-    <row r="9" spans="1:3" ht="15.75">
-      <c r="A9" s="20"/>
-      <c r="B9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="16"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75">
-      <c r="A10" s="20"/>
-      <c r="B10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="16"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="20"/>
-      <c r="B11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="16"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="20"/>
-      <c r="B12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="16"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="20"/>
-      <c r="B13" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="17"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75">
-      <c r="A14" s="20"/>
-      <c r="B14" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="C24" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75">
+      <c r="A25" s="21"/>
+      <c r="B25" s="24" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75">
-      <c r="A15" s="20"/>
-      <c r="B15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75">
-      <c r="A16" s="20"/>
-      <c r="B16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="18"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.75">
-      <c r="A17" s="20"/>
-      <c r="B17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="18"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75">
-      <c r="A18" s="20"/>
-      <c r="B18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="18"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75">
-      <c r="A19" s="20"/>
-      <c r="B19" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="18"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75">
-      <c r="A20" s="20"/>
-      <c r="B20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="18"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75">
-      <c r="A21" s="20"/>
-      <c r="B21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="18"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75">
-      <c r="A22" s="20"/>
-      <c r="B22" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="18"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75">
-      <c r="A23" s="20"/>
-      <c r="B23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="18"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="6" t="s">
+      <c r="C25" s="20"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75">
+      <c r="A26" s="21"/>
+      <c r="B26" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="6" t="s">
+      <c r="C26" s="20"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75">
+      <c r="A27" s="21"/>
+      <c r="B27" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="19"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="19"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="19"/>
+      <c r="C27" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2106,27 +2160,27 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2137,10 +2191,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection sqref="A1:A26"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2148,134 +2202,177 @@
     <col min="1" max="1" width="74.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75">
+      <c r="A3" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
+      <c r="A6" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75">
+      <c r="A8" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75">
-      <c r="A2" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75">
-      <c r="A3" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75">
-      <c r="A4" s="2" t="s">
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="A9" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75">
-      <c r="A5" s="2" t="s">
+    <row r="10" spans="1:3" ht="15.75">
+      <c r="A10" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75">
-      <c r="A6" s="2" t="s">
+    <row r="11" spans="1:3" ht="15.75">
+      <c r="A11" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75">
-      <c r="A7" s="2" t="s">
+    <row r="12" spans="1:3" ht="15.75">
+      <c r="A12" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75">
-      <c r="A8" s="2" t="s">
+    <row r="13" spans="1:3" ht="15.75">
+      <c r="A13" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75">
+      <c r="A14" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75">
-      <c r="A9" s="2" t="s">
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="A16" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75">
-      <c r="A10" s="2" t="s">
+    <row r="17" spans="1:1" ht="15.75">
+      <c r="A17" s="2" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.75">
-      <c r="A11" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.75">
-      <c r="A12" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.75">
-      <c r="A13" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="15.75">
-      <c r="A14" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.75">
-      <c r="A15" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="15.75">
-      <c r="A16" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75">
-      <c r="A17" s="12" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75">
       <c r="A18" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75">
+      <c r="A19" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75">
+      <c r="A20" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75">
+      <c r="A21" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75">
+      <c r="A22" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75">
+      <c r="A23" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75">
+      <c r="A24" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75">
+      <c r="A25" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75">
+      <c r="A26" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75">
-      <c r="A19" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75">
-      <c r="A20" s="11" t="s">
+    <row r="27" spans="1:1" ht="15.75">
+      <c r="A27" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75">
-      <c r="A21" s="11" t="s">
+    <row r="28" spans="1:1" ht="15.75">
+      <c r="A28" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75">
-      <c r="A22" s="11" t="s">
+    <row r="29" spans="1:1" ht="15.75">
+      <c r="A29" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.75">
-      <c r="A23" s="11" t="s">
+    <row r="30" spans="1:1" ht="15.75">
+      <c r="A30" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.75">
+      <c r="A31" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.75">
+      <c r="A32" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.75">
+      <c r="A33" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75">
-      <c r="A24" s="11" t="s">
+    <row r="34" spans="1:1" ht="15.75">
+      <c r="A34" s="7" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="15.75">
-      <c r="A25" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.75">
-      <c r="A26" s="11" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2290,13 +2387,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5703125" customWidth="1"/>
     <col min="4" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
@@ -2304,243 +2401,246 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" t="s">
         <v>140</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>141</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>142</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>143</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>144</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>145</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>146</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="30">
+      <c r="A2" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B2" s="10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="30">
-      <c r="A2" s="21" t="s">
+      <c r="C2" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="D2" t="s">
         <v>150</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>151</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="12"/>
+      <c r="C3" t="s">
         <v>152</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="12"/>
+      <c r="C4" t="s">
         <v>153</v>
       </c>
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="B3" s="24"/>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="12"/>
+      <c r="C5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="B4" s="24"/>
-      <c r="C4" t="s">
+    <row r="6" spans="1:9">
+      <c r="B6" s="12"/>
+      <c r="C6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="B5" s="24"/>
-      <c r="C5" t="s">
+    <row r="7" spans="1:9">
+      <c r="B7" s="12"/>
+      <c r="C7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="B6" s="24"/>
-      <c r="C6" t="s">
+    <row r="8" spans="1:9">
+      <c r="B8" s="12"/>
+      <c r="C8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="B7" s="24"/>
-      <c r="C7" t="s">
+    <row r="9" spans="1:9">
+      <c r="B9" s="12"/>
+      <c r="C9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="B8" s="24"/>
-      <c r="C8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="B9" s="24"/>
-      <c r="C9" t="s">
-        <v>160</v>
-      </c>
-    </row>
     <row r="10" spans="1:9">
-      <c r="B10" s="24"/>
+      <c r="B10" s="12"/>
       <c r="C10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="B11" s="24"/>
+      <c r="B11" s="12"/>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="B12" s="24"/>
+      <c r="B12" s="12"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="B13" s="21" t="s">
-        <v>162</v>
+      <c r="B13" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="C13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" t="s">
         <v>151</v>
-      </c>
-      <c r="D13" t="s">
-        <v>152</v>
-      </c>
-      <c r="E13" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="C14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="C15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="C16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="C17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="C18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
-      <c r="C17" t="s">
+    <row r="19" spans="2:9">
+      <c r="C19" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
-      <c r="C18" t="s">
+    <row r="20" spans="2:9">
+      <c r="C20" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
-      <c r="C19" s="21" t="s">
+    <row r="21" spans="2:9">
+      <c r="C21" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
-      <c r="C20" t="s">
+    <row r="22" spans="2:9">
+      <c r="C22" s="9" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="C21" t="s">
+      <c r="I22" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="C23" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
-      <c r="C22" s="21" t="s">
+    <row r="24" spans="2:9">
+      <c r="C24" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
-      <c r="C23" t="s">
+    <row r="25" spans="2:9">
+      <c r="C25" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
-      <c r="C24" t="s">
+    <row r="26" spans="2:9">
+      <c r="C26" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
-      <c r="C25" t="s">
+    <row r="27" spans="2:9">
+      <c r="C27" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
-      <c r="C26" t="s">
+    <row r="31" spans="2:9">
+      <c r="B31" s="9" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="C27" t="s">
+      <c r="C31" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="C31" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:9">
       <c r="C32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="C33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="C34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="C35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="C36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="C37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="2:3">
       <c r="C38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="2:3">
       <c r="C39" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="2:3">
       <c r="C40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="2:3">
@@ -2549,61 +2649,61 @@
       </c>
     </row>
     <row r="43" spans="2:3">
-      <c r="B43" s="21" t="s">
-        <v>179</v>
+      <c r="B43" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="C43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="2:3">
       <c r="C44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="C45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="2:3">
       <c r="C46" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="C47" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="2:3">
       <c r="C48" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="C49" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="C50" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="C51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="C52" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="C53" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2613,1035 +2713,1035 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" t="s">
         <v>183</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
+        <v>150</v>
+      </c>
+      <c r="E56" t="s">
         <v>184</v>
       </c>
-      <c r="C56" t="s">
+      <c r="F56" t="s">
         <v>185</v>
       </c>
-      <c r="D56" t="s">
-        <v>152</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="G56" t="s">
         <v>186</v>
-      </c>
-      <c r="F56" t="s">
-        <v>187</v>
-      </c>
-      <c r="G56" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="C57" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="C58" t="s">
-        <v>190</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="C59" t="s">
-        <v>191</v>
+        <v>303</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="C60" t="s">
-        <v>192</v>
+        <v>304</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="C61" t="s">
-        <v>193</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="C62" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="C63" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="C64" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="2:7">
       <c r="C65" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="2:7">
       <c r="C66" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="2:7">
       <c r="C67" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="68" spans="2:7">
       <c r="C68" t="s">
-        <v>200</v>
+        <v>306</v>
       </c>
     </row>
     <row r="69" spans="2:7">
       <c r="C69" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="70" spans="2:7">
       <c r="C70" t="s">
-        <v>202</v>
+        <v>307</v>
       </c>
     </row>
     <row r="71" spans="2:7">
       <c r="C71" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="72" spans="2:7">
       <c r="C72" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="2:7">
       <c r="C73" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74" spans="2:7">
       <c r="C74" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="2:7">
       <c r="C75" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="2:7">
       <c r="B77" t="s">
-        <v>207</v>
-      </c>
-      <c r="C77" s="21" t="s">
-        <v>208</v>
+        <v>200</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>201</v>
       </c>
       <c r="D77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E77" t="s">
+        <v>184</v>
+      </c>
+      <c r="F77" t="s">
+        <v>185</v>
+      </c>
+      <c r="G77" t="s">
         <v>186</v>
       </c>
-      <c r="F77" t="s">
-        <v>187</v>
-      </c>
-      <c r="G77" t="s">
-        <v>188</v>
-      </c>
     </row>
     <row r="78" spans="2:7">
-      <c r="C78" s="21" t="s">
-        <v>209</v>
+      <c r="C78" s="9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="2:7">
       <c r="C79" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="80" spans="2:7">
       <c r="C80" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="82" spans="3:3">
-      <c r="C82" s="21" t="s">
-        <v>213</v>
+      <c r="C82" s="9" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" spans="3:3">
-      <c r="C86" s="21" t="s">
-        <v>214</v>
+      <c r="C86" s="9" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="3:3">
-      <c r="C91" s="21" t="s">
-        <v>215</v>
+      <c r="C91" s="9" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="C97" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="C98" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="C99" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="C100" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="B104" t="s">
-        <v>224</v>
-      </c>
-      <c r="C104" s="21" t="s">
-        <v>208</v>
+        <v>217</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="C105" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="C107" s="21" t="s">
-        <v>226</v>
+      <c r="C107" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="C108" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="C109" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="C110" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="C111" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="C112" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="113" spans="2:9">
       <c r="C113" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="114" spans="2:9">
       <c r="C114" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="115" spans="2:9">
       <c r="C115" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="116" spans="2:9">
       <c r="C116" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="117" spans="2:9">
       <c r="C117" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="119" spans="2:9">
       <c r="B119" t="s">
-        <v>232</v>
-      </c>
-      <c r="C119" s="21" t="s">
-        <v>208</v>
+        <v>225</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>201</v>
       </c>
       <c r="D119" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E119" t="s">
+        <v>184</v>
+      </c>
+      <c r="F119" t="s">
+        <v>185</v>
+      </c>
+      <c r="G119" t="s">
         <v>186</v>
       </c>
-      <c r="F119" t="s">
-        <v>187</v>
-      </c>
-      <c r="G119" t="s">
-        <v>188</v>
-      </c>
       <c r="H119" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="I119" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="120" spans="2:9">
       <c r="C120" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="121" spans="2:9">
       <c r="C121" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="122" spans="2:9">
       <c r="C122" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="123" spans="2:9">
       <c r="C123" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="124" spans="2:9">
       <c r="C124" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="126" spans="2:9">
-      <c r="C126" s="21" t="s">
-        <v>226</v>
+      <c r="C126" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="127" spans="2:9">
       <c r="C127" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="128" spans="2:9">
       <c r="C128" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="129" spans="2:9">
       <c r="C129" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="130" spans="2:9">
       <c r="C130" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="131" spans="2:9">
       <c r="C131" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="132" spans="2:9">
       <c r="C132" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="133" spans="2:9">
       <c r="C133" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="134" spans="2:9">
       <c r="C134" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="135" spans="2:9">
       <c r="C135" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="136" spans="2:9">
       <c r="C136" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="137" spans="2:9">
       <c r="C137" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="138" spans="2:9">
       <c r="C138" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="139" spans="2:9">
       <c r="C139" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="140" spans="2:9">
       <c r="C140" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="141" spans="2:9">
       <c r="C141" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="143" spans="2:9">
-      <c r="B143" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="C143" s="21" t="s">
-        <v>249</v>
+      <c r="B143" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>242</v>
       </c>
       <c r="D143" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E143" t="s">
+        <v>184</v>
+      </c>
+      <c r="F143" t="s">
+        <v>184</v>
+      </c>
+      <c r="G143" t="s">
         <v>186</v>
       </c>
-      <c r="F143" t="s">
-        <v>186</v>
-      </c>
-      <c r="G143" t="s">
-        <v>188</v>
-      </c>
       <c r="H143" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I143" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="144" spans="2:9">
       <c r="C144" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="145" spans="3:3">
       <c r="C145" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="146" spans="3:3">
       <c r="C146" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="147" spans="3:3">
       <c r="C147" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="148" spans="3:3">
       <c r="C148" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="149" spans="3:3">
       <c r="C149" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="151" spans="3:3">
-      <c r="C151" s="21" t="s">
-        <v>226</v>
+      <c r="C151" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="152" spans="3:3">
       <c r="C152" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="153" spans="3:3">
       <c r="C153" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="154" spans="3:3">
       <c r="C154" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="155" spans="3:3">
       <c r="C155" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="156" spans="3:3">
       <c r="C156" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="157" spans="3:3">
       <c r="C157" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="158" spans="3:3">
       <c r="C158" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="159" spans="3:3">
       <c r="C159" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9">
+      <c r="A161" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B161" s="9" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="161" spans="1:9">
-      <c r="A161" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="B161" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="C161" s="21" t="s">
-        <v>249</v>
+      <c r="C161" s="9" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="C162" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="C163" t="s">
-        <v>256</v>
+        <v>308</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="C164" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="C165" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="C166" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="168" spans="1:9">
-      <c r="C168" s="21" t="s">
-        <v>226</v>
+      <c r="C168" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="C169" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="171" spans="1:9">
-      <c r="B171" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="C171" s="21" t="s">
-        <v>249</v>
+      <c r="B171" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C171" s="9" t="s">
+        <v>242</v>
       </c>
       <c r="D171" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E171" t="s">
+        <v>184</v>
+      </c>
+      <c r="F171" t="s">
+        <v>184</v>
+      </c>
+      <c r="G171" t="s">
         <v>186</v>
       </c>
-      <c r="F171" t="s">
-        <v>186</v>
-      </c>
-      <c r="G171" t="s">
-        <v>188</v>
-      </c>
       <c r="H171" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I171" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="172" spans="1:9">
-      <c r="C172" s="25" t="s">
-        <v>262</v>
+      <c r="C172" s="13" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="173" spans="1:9">
       <c r="C173" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="C174" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="C175" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="C176" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="177" spans="3:3">
-      <c r="C177" s="21"/>
+      <c r="C177" s="9"/>
     </row>
     <row r="178" spans="3:3">
-      <c r="C178" s="21" t="s">
-        <v>226</v>
+      <c r="C178" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="179" spans="3:3">
       <c r="C179" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="180" spans="3:3">
       <c r="C180" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="181" spans="3:3">
       <c r="C181" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="182" spans="3:3">
       <c r="C182" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="183" spans="3:3">
       <c r="C183" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="184" spans="3:3">
       <c r="C184" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="185" spans="3:3">
       <c r="C185" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="186" spans="3:3">
       <c r="C186" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="187" spans="3:3">
       <c r="C187" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="188" spans="3:3">
       <c r="C188" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="189" spans="3:3">
       <c r="C189" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="190" spans="3:3">
       <c r="C190" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="191" spans="3:3">
       <c r="C191" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="192" spans="3:3">
       <c r="C192" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="193" spans="2:9">
       <c r="C193" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="194" spans="2:9">
       <c r="C194" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="195" spans="2:9">
       <c r="C195" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="196" spans="2:9">
       <c r="C196" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="197" spans="2:9">
       <c r="C197" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="198" spans="2:9">
       <c r="C198" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="200" spans="2:9">
-      <c r="B200" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="C200" s="21" t="s">
-        <v>249</v>
+      <c r="B200" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C200" s="9" t="s">
+        <v>242</v>
       </c>
       <c r="D200" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E200" t="s">
+        <v>184</v>
+      </c>
+      <c r="F200" t="s">
+        <v>184</v>
+      </c>
+      <c r="G200" t="s">
         <v>186</v>
       </c>
-      <c r="F200" t="s">
-        <v>186</v>
-      </c>
-      <c r="G200" t="s">
-        <v>188</v>
-      </c>
       <c r="H200" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I200" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="201" spans="2:9">
       <c r="C201" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="202" spans="2:9">
       <c r="C202" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="203" spans="2:9">
       <c r="C203" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="204" spans="2:9">
       <c r="C204" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="205" spans="2:9">
       <c r="C205" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="207" spans="2:9">
-      <c r="C207" s="21" t="s">
-        <v>226</v>
+      <c r="C207" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="208" spans="2:9">
       <c r="C208" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="209" spans="2:9">
       <c r="C209" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="210" spans="2:9">
       <c r="C210" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="211" spans="2:9">
       <c r="C211" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="212" spans="2:9">
       <c r="C212" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="213" spans="2:9">
       <c r="C213" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="214" spans="2:9">
       <c r="C214" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="215" spans="2:9">
       <c r="C215" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="217" spans="2:9">
-      <c r="B217" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="C217" s="21" t="s">
-        <v>249</v>
+      <c r="B217" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C217" s="9" t="s">
+        <v>242</v>
       </c>
       <c r="D217" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E217" t="s">
+        <v>184</v>
+      </c>
+      <c r="F217" t="s">
+        <v>184</v>
+      </c>
+      <c r="G217" t="s">
         <v>186</v>
       </c>
-      <c r="F217" t="s">
-        <v>186</v>
-      </c>
-      <c r="G217" t="s">
-        <v>188</v>
-      </c>
       <c r="H217" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I217" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="218" spans="2:9">
       <c r="C218" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="219" spans="2:9">
       <c r="C219" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="220" spans="2:9">
       <c r="C220" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="221" spans="2:9">
       <c r="C221" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="223" spans="2:9">
-      <c r="C223" s="21" t="s">
-        <v>226</v>
+      <c r="C223" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="224" spans="2:9">
       <c r="C224" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="225" spans="2:3">
       <c r="C225" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="226" spans="2:3">
       <c r="C226" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="227" spans="2:3">
       <c r="C227" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="228" spans="2:3">
       <c r="C228" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="229" spans="2:3">
       <c r="C229" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="230" spans="2:3">
       <c r="C230" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="231" spans="2:3">
       <c r="C231" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="232" spans="2:3">
       <c r="C232" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="234" spans="2:3">
       <c r="B234" t="s">
-        <v>292</v>
-      </c>
-      <c r="C234" s="21" t="s">
-        <v>249</v>
+        <v>284</v>
+      </c>
+      <c r="C234" s="9" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="235" spans="2:3">
       <c r="C235" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="236" spans="2:3">
       <c r="C236" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="237" spans="2:3">
       <c r="C237" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="238" spans="2:3">
       <c r="C238" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="240" spans="2:3">
-      <c r="C240" s="21" t="s">
-        <v>226</v>
+      <c r="C240" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="241" spans="3:3">
       <c r="C241" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="242" spans="3:3">
       <c r="C242" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="243" spans="3:3">
       <c r="C243" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="244" spans="3:3">
       <c r="C244" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="245" spans="3:3">
       <c r="C245" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="246" spans="3:3">
       <c r="C246" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="247" spans="3:3">
       <c r="C247" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="248" spans="3:3">
       <c r="C248" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="249" spans="3:3">
       <c r="C249" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="250" spans="3:3">
       <c r="C250" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>